<commit_message>
added 10 percent change in output
</commit_message>
<xml_diff>
--- a/analysis/sensitivity/sensitivityOutput.xlsx
+++ b/analysis/sensitivity/sensitivityOutput.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>Total.water.demand</t>
   </si>
@@ -143,6 +143,36 @@
   </si>
   <si>
     <t>Staff hiring</t>
+  </si>
+  <si>
+    <t>hiring_of_staff_min_10perc.csv</t>
+  </si>
+  <si>
+    <t>hiring_of_staff_plus_10perc.csv</t>
+  </si>
+  <si>
+    <t>income_flow_min_10perc.csv</t>
+  </si>
+  <si>
+    <t>income_flow_plus_10perc.csv</t>
+  </si>
+  <si>
+    <t>infrastructure_aging_min_10perc.csv</t>
+  </si>
+  <si>
+    <t>infrastructure_aging_plus_10perc.csv</t>
+  </si>
+  <si>
+    <t>maintenance_expenditures_min_10perc.csv</t>
+  </si>
+  <si>
+    <t>maintenance_expenditures_plus_10perc.csv</t>
+  </si>
+  <si>
+    <t>staff_leaving_min_10perc.csv</t>
+  </si>
+  <si>
+    <t>staff_leaving_plus_10perc.csv</t>
   </si>
 </sst>
 </file>
@@ -971,10 +1001,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:G49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1039,19 +1069,19 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>6.0386784321636799E-2</v>
+        <v>6.0386783999999999E-2</v>
       </c>
       <c r="D3">
-        <v>2.91493822200206E-2</v>
+        <v>2.9149382000000001E-2</v>
       </c>
       <c r="E3">
-        <v>4.7266211045612697E-2</v>
+        <v>4.7266211000000002E-2</v>
       </c>
       <c r="F3">
-        <v>4.5159585271897298E-2</v>
+        <v>4.5159585000000002E-2</v>
       </c>
       <c r="G3">
-        <v>5.2526200019247403E-3</v>
+        <v>5.2526200000000004E-3</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1062,19 +1092,19 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>5.9770877692691501E-2</v>
+        <v>5.9770878E-2</v>
       </c>
       <c r="D4">
-        <v>2.8797197512325901E-2</v>
+        <v>2.8797198E-2</v>
       </c>
       <c r="E4">
-        <v>5.5773505200775703E-2</v>
+        <v>5.5773505000000001E-2</v>
       </c>
       <c r="F4">
-        <v>5.3660390732816803E-2</v>
+        <v>5.3660391000000002E-2</v>
       </c>
       <c r="G4">
-        <v>5.1605994404950398E-3</v>
+        <v>5.1605990000000001E-3</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1082,22 +1112,22 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>6.3218106403634705E-2</v>
+        <v>6.3218105999999996E-2</v>
       </c>
       <c r="C5">
-        <v>0.14600445160653699</v>
+        <v>0.14600445200000001</v>
       </c>
       <c r="D5">
-        <v>7.1973219901821803E-2</v>
+        <v>7.1973220000000004E-2</v>
       </c>
       <c r="E5">
-        <v>0.27718088907446697</v>
+        <v>0.27718088899999999</v>
       </c>
       <c r="F5">
-        <v>0.230678488283314</v>
+        <v>0.23067848799999999</v>
       </c>
       <c r="G5">
-        <v>0.20442770816908701</v>
+        <v>0.20442770800000001</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1105,22 +1135,22 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>6.2228581831650899E-2</v>
+        <v>6.2228581999999998E-2</v>
       </c>
       <c r="C6">
-        <v>0.14346047657859201</v>
+        <v>0.143460477</v>
       </c>
       <c r="D6">
-        <v>7.1051792848490294E-2</v>
+        <v>7.1051793000000002E-2</v>
       </c>
       <c r="E6">
-        <v>0.21710934912284099</v>
+        <v>0.21710934900000001</v>
       </c>
       <c r="F6">
-        <v>0.17459152181101301</v>
+        <v>0.174591522</v>
       </c>
       <c r="G6">
-        <v>0.25876085972696</v>
+        <v>0.25876085999999998</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1128,22 +1158,22 @@
         <v>10</v>
       </c>
       <c r="B7">
-        <v>0.296295542149425</v>
+        <v>0.29629554200000002</v>
       </c>
       <c r="C7">
-        <v>0.33865164868223102</v>
+        <v>0.338651649</v>
       </c>
       <c r="D7">
-        <v>0.166344498916321</v>
+        <v>0.16634449900000001</v>
       </c>
       <c r="E7">
-        <v>0.52006118972635895</v>
+        <v>0.52006118999999995</v>
       </c>
       <c r="F7">
-        <v>0.43458874302560802</v>
+        <v>0.434588743</v>
       </c>
       <c r="G7">
-        <v>0.72641330160357698</v>
+        <v>0.72641330199999998</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1151,22 +1181,22 @@
         <v>11</v>
       </c>
       <c r="B8">
-        <v>0.291392696062237</v>
+        <v>0.29139269600000001</v>
       </c>
       <c r="C8">
-        <v>0.34423825865596802</v>
+        <v>0.34423825899999999</v>
       </c>
       <c r="D8">
-        <v>0.167202023206105</v>
+        <v>0.16720202300000001</v>
       </c>
       <c r="E8">
-        <v>0.832692249792373</v>
+        <v>0.83269225000000002</v>
       </c>
       <c r="F8">
-        <v>0.73018092508157795</v>
+        <v>0.73018092499999998</v>
       </c>
       <c r="G8">
-        <v>0.53483794641384597</v>
+        <v>0.53483794600000001</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1174,22 +1204,22 @@
         <v>12</v>
       </c>
       <c r="B9">
-        <v>8.1836888538442107E-2</v>
+        <v>8.1836888999999996E-2</v>
       </c>
       <c r="C9">
-        <v>2.7326230273990601E-2</v>
+        <v>2.732623E-2</v>
       </c>
       <c r="D9">
-        <v>1.31763826562716E-2</v>
+        <v>1.3176383E-2</v>
       </c>
       <c r="E9">
-        <v>6.9717234898745706E-2</v>
+        <v>6.9717235000000002E-2</v>
       </c>
       <c r="F9">
-        <v>6.3528169931990799E-2</v>
+        <v>6.3528169999999995E-2</v>
       </c>
       <c r="G9">
-        <v>0.10291390897147799</v>
+        <v>0.102913909</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1197,22 +1227,22 @@
         <v>13</v>
       </c>
       <c r="B10">
-        <v>8.1613148015724404E-2</v>
+        <v>8.1613147999999996E-2</v>
       </c>
       <c r="C10">
-        <v>2.7465437578033301E-2</v>
+        <v>2.7465437999999998E-2</v>
       </c>
       <c r="D10">
-        <v>1.32170163985632E-2</v>
+        <v>1.3217016E-2</v>
       </c>
       <c r="E10">
-        <v>8.6915223763523494E-2</v>
+        <v>8.6915223999999999E-2</v>
       </c>
       <c r="F10">
-        <v>8.0648664415919696E-2</v>
+        <v>8.0648663999999995E-2</v>
       </c>
       <c r="G10">
-        <v>0.10205919915098401</v>
+        <v>0.102059199</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1220,22 +1250,22 @@
         <v>14</v>
       </c>
       <c r="B11">
-        <v>0.122391942025593</v>
+        <v>0.122391942</v>
       </c>
       <c r="C11">
-        <v>0.18770721797147899</v>
+        <v>0.18770721800000001</v>
       </c>
       <c r="D11">
-        <v>9.2044160542087194E-2</v>
+        <v>9.2044160999999999E-2</v>
       </c>
       <c r="E11">
-        <v>0.31509109222841802</v>
+        <v>0.31509109200000002</v>
       </c>
       <c r="F11">
-        <v>0.26766622890259301</v>
+        <v>0.26766622899999998</v>
       </c>
       <c r="G11">
-        <v>0.33536207346005797</v>
+        <v>0.33536207299999998</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1243,516 +1273,758 @@
         <v>15</v>
       </c>
       <c r="B12">
-        <v>0.121489224394038</v>
+        <v>0.12148922400000001</v>
       </c>
       <c r="C12">
-        <v>0.189500916429927</v>
+        <v>0.18950091599999999</v>
       </c>
       <c r="D12">
-        <v>9.2364830889952704E-2</v>
+        <v>9.2364830999999994E-2</v>
       </c>
       <c r="E12">
-        <v>0.46371053304863102</v>
+        <v>0.46371053299999998</v>
       </c>
       <c r="F12">
-        <v>0.41132833202270602</v>
+        <v>0.41132833200000002</v>
       </c>
       <c r="G12">
-        <v>0.27232888655467802</v>
+        <v>0.27232888700000002</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="B13">
         <v>0</v>
       </c>
       <c r="C13">
-        <v>0.20956815196741299</v>
+        <v>1.9450076119999999</v>
       </c>
       <c r="D13">
-        <v>0.101217496444493</v>
+        <v>0.96887429199999997</v>
       </c>
       <c r="E13">
-        <v>0.32571946077836</v>
+        <v>1.964753741</v>
       </c>
       <c r="F13">
-        <v>0.32377413515805098</v>
+        <v>1.9704729679999999</v>
       </c>
       <c r="G13">
-        <v>4.9186866783564397E-2</v>
+        <v>0.93650194600000003</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14">
         <v>0</v>
       </c>
       <c r="C14">
-        <v>0.213653794063732</v>
+        <v>0.20956815200000001</v>
       </c>
       <c r="D14">
-        <v>0.10244670160515799</v>
+        <v>0.101217496</v>
       </c>
       <c r="E14">
-        <v>0.53539510915023902</v>
+        <v>0.32571946099999999</v>
       </c>
       <c r="F14">
-        <v>0.53263053866563703</v>
+        <v>0.32377413500000002</v>
       </c>
       <c r="G14">
-        <v>4.5290634498528402E-2</v>
+        <v>4.9186867000000002E-2</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="B15">
         <v>0</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>2.3177102230000002</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>1.071649635</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>5.4481982020000004</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>5.3781658109999997</v>
       </c>
       <c r="G15">
-        <v>0</v>
+        <v>0.37484250099999999</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B16">
         <v>0</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>0.21365379400000001</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>0.102446702</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>0.53539510899999998</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <v>0.53263053900000001</v>
       </c>
       <c r="G16">
-        <v>0</v>
+        <v>4.5290634000000003E-2</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B17">
         <v>0</v>
       </c>
       <c r="C17">
-        <v>0.130185043792439</v>
+        <v>0</v>
       </c>
       <c r="D17">
-        <v>0.62964842711375102</v>
+        <v>0</v>
       </c>
       <c r="E17">
-        <v>0.23042215706652799</v>
+        <v>0</v>
       </c>
       <c r="F17">
-        <v>0.14509060769440801</v>
+        <v>0</v>
       </c>
       <c r="G17">
-        <v>0.48171799240838598</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B18">
         <v>0</v>
       </c>
       <c r="C18">
-        <v>0.136383035339147</v>
+        <v>0</v>
       </c>
       <c r="D18">
-        <v>0.631088186186051</v>
+        <v>0</v>
       </c>
       <c r="E18">
-        <v>0.26890199129167802</v>
+        <v>0</v>
       </c>
       <c r="F18">
-        <v>0.17317315264099001</v>
+        <v>0</v>
       </c>
       <c r="G18">
-        <v>0.22368235656684299</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="B19">
         <v>0</v>
       </c>
       <c r="C19">
-        <v>2.3915298769308699</v>
+        <v>1.043357251</v>
       </c>
       <c r="D19">
-        <v>0.97230575361775895</v>
+        <v>6.2148036280000003</v>
       </c>
       <c r="E19">
-        <v>1.0478576111146001</v>
+        <v>1.584611649</v>
       </c>
       <c r="F19">
-        <v>0.96072294395753</v>
+        <v>0.98099452099999995</v>
       </c>
       <c r="G19">
-        <v>0.26246611515766499</v>
+        <v>11.63870794</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B20">
         <v>0</v>
       </c>
       <c r="C20">
-        <v>2.2422492948916899</v>
+        <v>0.130185044</v>
       </c>
       <c r="D20">
-        <v>0.99347782223717895</v>
+        <v>0.62964842700000001</v>
       </c>
       <c r="E20">
-        <v>0.60571649904347402</v>
+        <v>0.23042215699999999</v>
       </c>
       <c r="F20">
-        <v>0.53242664162588604</v>
+        <v>0.14509060800000001</v>
       </c>
       <c r="G20">
-        <v>0.388746756370911</v>
+        <v>0.48171799199999998</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="B21">
         <v>0</v>
       </c>
       <c r="C21">
-        <v>0.15027947394910099</v>
+        <v>1.676265503</v>
       </c>
       <c r="D21">
-        <v>0.492148957641109</v>
+        <v>6.3614307280000002</v>
       </c>
       <c r="E21">
-        <v>0.29330633955471003</v>
+        <v>4.3111793550000002</v>
       </c>
       <c r="F21">
-        <v>0.18686387608711899</v>
+        <v>2.3210746809999998</v>
       </c>
       <c r="G21">
-        <v>0.23069133255511301</v>
+        <v>0.97645457800000002</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B22">
         <v>0</v>
       </c>
       <c r="C22">
-        <v>0.14121863898872</v>
+        <v>0.13638303500000001</v>
       </c>
       <c r="D22">
-        <v>0.48304491983591002</v>
+        <v>0.63108818600000005</v>
       </c>
       <c r="E22">
-        <v>0.24619357972056599</v>
+        <v>0.26890199100000001</v>
       </c>
       <c r="F22">
-        <v>0.15265962459729601</v>
+        <v>0.173173153</v>
       </c>
       <c r="G22">
-        <v>0.49474369985703598</v>
+        <v>0.223682357</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="B23">
         <v>0</v>
       </c>
       <c r="C23">
-        <v>7.8525300268299694E-2</v>
+        <v>32.798069269999999</v>
       </c>
       <c r="D23">
-        <v>3.76700525317024E-2</v>
+        <v>8.7926528309999998</v>
       </c>
       <c r="E23">
-        <v>6.0933182123777199E-2</v>
+        <v>12.19495963</v>
       </c>
       <c r="F23">
-        <v>5.96911513555358E-2</v>
+        <v>10.26898342</v>
       </c>
       <c r="G23">
-        <v>7.4707961626460503E-3</v>
+        <v>1.664558931</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B24">
         <v>0</v>
       </c>
       <c r="C24">
-        <v>7.8731135479662304E-2</v>
+        <v>2.391529877</v>
       </c>
       <c r="D24">
-        <v>3.7687275911614297E-2</v>
+        <v>0.97230575399999997</v>
       </c>
       <c r="E24">
-        <v>7.5244405912679599E-2</v>
+        <v>1.047857611</v>
       </c>
       <c r="F24">
-        <v>7.4019145436852493E-2</v>
+        <v>0.96072294400000002</v>
       </c>
       <c r="G24">
-        <v>7.4640482215112998E-3</v>
+        <v>0.262466115</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="B25">
-        <v>0.10303139550266301</v>
+        <v>0</v>
       </c>
       <c r="C25">
-        <v>0.126654296203463</v>
+        <v>17.199897910000001</v>
       </c>
       <c r="D25">
-        <v>6.17724923363831E-2</v>
+        <v>10.83267603</v>
       </c>
       <c r="E25">
-        <v>0.30294431871854499</v>
+        <v>3.373289599</v>
       </c>
       <c r="F25">
-        <v>0.26724912930988298</v>
+        <v>2.9560069790000001</v>
       </c>
       <c r="G25">
-        <v>0.213314990767319</v>
+        <v>11.82325301</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B26">
-        <v>0.10354295451860999</v>
+        <v>0</v>
       </c>
       <c r="C26">
-        <v>0.125765191377188</v>
+        <v>2.2422492950000001</v>
       </c>
       <c r="D26">
-        <v>6.1583833626926099E-2</v>
+        <v>0.99347782200000001</v>
       </c>
       <c r="E26">
-        <v>0.220157899920739</v>
+        <v>0.60571649900000002</v>
       </c>
       <c r="F26">
-        <v>0.18681607292659699</v>
+        <v>0.53242664200000001</v>
       </c>
       <c r="G26">
-        <v>0.24421637719540201</v>
+        <v>0.38874675600000003</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="B27">
-        <v>0.19674588488491301</v>
+        <v>0</v>
       </c>
       <c r="C27">
-        <v>6.60819087622182E-2</v>
+        <v>2.0167843470000002</v>
       </c>
       <c r="D27">
-        <v>3.1786775856872097E-2</v>
+        <v>5.3808147020000003</v>
       </c>
       <c r="E27">
-        <v>0.20986254176444699</v>
+        <v>5.3985509990000002</v>
       </c>
       <c r="F27">
-        <v>0.19446486009985001</v>
+        <v>2.7921400680000001</v>
       </c>
       <c r="G27">
-        <v>0.24557069771190401</v>
+        <v>1.072434122</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B28">
-        <v>0.198157767148845</v>
+        <v>0</v>
       </c>
       <c r="C28">
-        <v>6.5583800046676799E-2</v>
+        <v>0.150279474</v>
       </c>
       <c r="D28">
-        <v>3.1610433319198002E-2</v>
+        <v>0.49214895800000003</v>
       </c>
       <c r="E28">
-        <v>0.148013419942187</v>
+        <v>0.29330634</v>
       </c>
       <c r="F28">
-        <v>0.13318447868306399</v>
+        <v>0.18686387600000001</v>
       </c>
       <c r="G28">
-        <v>0.24998668220694001</v>
+        <v>0.230691333</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="B29">
-        <v>2.3719691577742001E-2</v>
+        <v>0</v>
       </c>
       <c r="C29">
-        <v>3.6984760474721601E-2</v>
+        <v>1.0914040039999999</v>
       </c>
       <c r="D29">
-        <v>1.80632831773932E-2</v>
+        <v>4.4545296790000002</v>
       </c>
       <c r="E29">
-        <v>9.0102020402723207E-2</v>
+        <v>1.6222213320000001</v>
       </c>
       <c r="F29">
-        <v>8.0361370189354298E-2</v>
+        <v>0.98142656699999997</v>
       </c>
       <c r="G29">
-        <v>6.0697061777872499E-2</v>
+        <v>11.17007173</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B30">
-        <v>2.3737593032836901E-2</v>
+        <v>0</v>
       </c>
       <c r="C30">
-        <v>3.6639030330769297E-2</v>
+        <v>0.14121863900000001</v>
       </c>
       <c r="D30">
-        <v>1.7938287931847902E-2</v>
+        <v>0.48304491999999999</v>
       </c>
       <c r="E30">
-        <v>7.5343121211294495E-2</v>
+        <v>0.24619358</v>
       </c>
       <c r="F30">
-        <v>6.5701509988305998E-2</v>
+        <v>0.15265962499999999</v>
       </c>
       <c r="G30">
-        <v>6.2655579758682495E-2</v>
+        <v>0.49474370000000001</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B31">
         <v>0</v>
       </c>
       <c r="C31">
-        <v>0.35236267080148698</v>
+        <v>7.8525300000000006E-2</v>
       </c>
       <c r="D31">
-        <v>0.16867485794727399</v>
+        <v>3.7670053000000002E-2</v>
       </c>
       <c r="E31">
-        <v>0.83995614770735405</v>
+        <v>6.0933182000000002E-2</v>
       </c>
       <c r="F31">
-        <v>0.83568812961245698</v>
+        <v>5.9691150999999998E-2</v>
       </c>
       <c r="G31">
-        <v>7.5913999239260899E-2</v>
+        <v>7.470796E-3</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>27</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>7.8731134999999994E-2</v>
+      </c>
+      <c r="D32">
+        <v>3.7687275999999999E-2</v>
+      </c>
+      <c r="E32">
+        <v>7.5244406E-2</v>
+      </c>
+      <c r="F32">
+        <v>7.4019144999999995E-2</v>
+      </c>
+      <c r="G32">
+        <v>7.464048E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>28</v>
+      </c>
+      <c r="B33">
+        <v>0.103031396</v>
+      </c>
+      <c r="C33">
+        <v>0.126654296</v>
+      </c>
+      <c r="D33">
+        <v>6.1772491999999998E-2</v>
+      </c>
+      <c r="E33">
+        <v>0.30294431900000002</v>
+      </c>
+      <c r="F33">
+        <v>0.26724912899999997</v>
+      </c>
+      <c r="G33">
+        <v>0.21331499100000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>29</v>
+      </c>
+      <c r="B34">
+        <v>0.10354295500000001</v>
+      </c>
+      <c r="C34">
+        <v>0.125765191</v>
+      </c>
+      <c r="D34">
+        <v>6.1583833999999997E-2</v>
+      </c>
+      <c r="E34">
+        <v>0.22015789999999999</v>
+      </c>
+      <c r="F34">
+        <v>0.186816073</v>
+      </c>
+      <c r="G34">
+        <v>0.24421637700000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>30</v>
+      </c>
+      <c r="B35">
+        <v>0.19674588500000001</v>
+      </c>
+      <c r="C35">
+        <v>6.6081908999999994E-2</v>
+      </c>
+      <c r="D35">
+        <v>3.1786776000000003E-2</v>
+      </c>
+      <c r="E35">
+        <v>0.20986254200000001</v>
+      </c>
+      <c r="F35">
+        <v>0.19446485999999999</v>
+      </c>
+      <c r="G35">
+        <v>0.245570698</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>31</v>
+      </c>
+      <c r="B36">
+        <v>0.19815776700000001</v>
+      </c>
+      <c r="C36">
+        <v>6.5583799999999998E-2</v>
+      </c>
+      <c r="D36">
+        <v>3.1610433E-2</v>
+      </c>
+      <c r="E36">
+        <v>0.14801342000000001</v>
+      </c>
+      <c r="F36">
+        <v>0.13318447899999999</v>
+      </c>
+      <c r="G36">
+        <v>0.24998668199999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>32</v>
+      </c>
+      <c r="B37">
+        <v>2.3719692000000001E-2</v>
+      </c>
+      <c r="C37">
+        <v>3.6984759999999998E-2</v>
+      </c>
+      <c r="D37">
+        <v>1.8063282999999999E-2</v>
+      </c>
+      <c r="E37">
+        <v>9.0102020000000005E-2</v>
+      </c>
+      <c r="F37">
+        <v>8.0361370000000001E-2</v>
+      </c>
+      <c r="G37">
+        <v>6.0697062000000003E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>33</v>
+      </c>
+      <c r="B38">
+        <v>2.3737593000000001E-2</v>
+      </c>
+      <c r="C38">
+        <v>3.6639030000000003E-2</v>
+      </c>
+      <c r="D38">
+        <v>1.7938288E-2</v>
+      </c>
+      <c r="E38">
+        <v>7.5343120999999999E-2</v>
+      </c>
+      <c r="F38">
+        <v>6.5701510000000005E-2</v>
+      </c>
+      <c r="G38">
+        <v>6.2655580000000002E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>51</v>
+      </c>
+      <c r="B39">
+        <v>0</v>
+      </c>
+      <c r="C39">
+        <v>4.1782543820000004</v>
+      </c>
+      <c r="D39">
+        <v>1.8750164069999999</v>
+      </c>
+      <c r="E39">
+        <v>9.1079623830000003</v>
+      </c>
+      <c r="F39">
+        <v>8.9236406600000002</v>
+      </c>
+      <c r="G39">
+        <v>0.60871179799999997</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>34</v>
+      </c>
+      <c r="B40">
+        <v>0</v>
+      </c>
+      <c r="C40">
+        <v>0.35236267100000002</v>
+      </c>
+      <c r="D40">
+        <v>0.16867485800000001</v>
+      </c>
+      <c r="E40">
+        <v>0.83995614799999996</v>
+      </c>
+      <c r="F40">
+        <v>0.83568812999999997</v>
+      </c>
+      <c r="G40">
+        <v>7.5913998999999996E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>52</v>
+      </c>
+      <c r="B41">
+        <v>0</v>
+      </c>
+      <c r="C41">
+        <v>2.9648739659999999</v>
+      </c>
+      <c r="D41">
+        <v>1.5047461099999999</v>
+      </c>
+      <c r="E41">
+        <v>2.6573316089999999</v>
+      </c>
+      <c r="F41">
+        <v>2.701344202</v>
+      </c>
+      <c r="G41">
+        <v>2.266152988</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>35</v>
       </c>
-      <c r="B32">
-        <v>0</v>
-      </c>
-      <c r="C32">
-        <v>0.34076812553797198</v>
-      </c>
-      <c r="D32">
-        <v>0.16511682702371699</v>
-      </c>
-      <c r="E32">
-        <v>0.47620610243309602</v>
-      </c>
-      <c r="F32">
-        <v>0.47415465168525101</v>
-      </c>
-      <c r="G32">
-        <v>8.8068326195827995E-2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="B42">
+        <v>0</v>
+      </c>
+      <c r="C42">
+        <v>0.340768126</v>
+      </c>
+      <c r="D42">
+        <v>0.16511682699999999</v>
+      </c>
+      <c r="E42">
+        <v>0.47620610200000002</v>
+      </c>
+      <c r="F42">
+        <v>0.47415465200000001</v>
+      </c>
+      <c r="G42">
+        <v>8.8068326000000002E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>42</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:G33 A35:A40">
+  <conditionalFormatting sqref="A44:A49 A3:B23 A1:G2">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H3:H12 C3:C22">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -1764,7 +2036,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H3:H32">
+  <conditionalFormatting sqref="B2:G42">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>